<commit_message>
update to 2.62 version of corridor for some programs #1-21 updated for slow T-LED drivers
Also, preparation for config.py file, that would hold few of the data together for quicker updates and distinction of corridor boxes, for now, there are 2 and extra 1 "unit" on my table
</commit_message>
<xml_diff>
--- a/HELPMEfile - MANUAL/tabulka programu.xlsx
+++ b/HELPMEfile - MANUAL/tabulka programu.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\novak\Documents\GitHub\LuxMeter\HELPMEfile - MANUAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C270E6-37F8-4094-950E-454733588E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6642B214-3968-4C95-8B38-59373A7ECF18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -25,8 +25,44 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Novák Michal</author>
+  </authors>
+  <commentList>
+    <comment ref="B24" authorId="0" shapeId="0" xr:uid="{2D866A38-93B0-4A0C-B0E4-4A2DB2F1FCD6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t>Novák Michal:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t xml:space="preserve">
+nepoužívat, byl tu nějaký duplikát, u zakázek pozor, kdyby se něco s P21 objevilo, prověřit.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="99">
   <si>
     <t>body pro vyplneni a postupne se bude "filtrovat seznam" mereni a když bude prazdne, tak tlacitko zalozit a pripravil by se novy program a cislo? + fajfka jestli je k tomu uz vytvoreny testovaci program?</t>
   </si>
@@ -295,17 +331,41 @@
     <t>FIN:0.7s, RON:180s/100%, FOUT:32s, ABL:15%, SOFF:/</t>
   </si>
   <si>
-    <t>nepoužívat, byl tu nějaký duplikát, u zakázek pozor, kdyby se něco s P21 objevilo, prověřit.</t>
-  </si>
-  <si>
     <t>FIN:0.7s, RON:120s/100%, FOUT:32s, ABL:0%, SOFF:/</t>
+  </si>
+  <si>
+    <t>5.0s</t>
+  </si>
+  <si>
+    <t>Program č. 28</t>
+  </si>
+  <si>
+    <t>FIN:0.7s, RON:60s/100%, FOUT:2s, ABL:10%, SOFF:1800s</t>
+  </si>
+  <si>
+    <t>0.7s,</t>
+  </si>
+  <si>
+    <t>60s/100%,</t>
+  </si>
+  <si>
+    <t>2s,</t>
+  </si>
+  <si>
+    <t>10%,</t>
+  </si>
+  <si>
+    <t>Program č. 29</t>
+  </si>
+  <si>
+    <t>FIN:5s, RON:300s/100%, FOUT:32s, ABL:10%, SOFF:/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -339,6 +399,21 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="2">
@@ -698,10 +773,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8636243C-025B-4E7E-AD67-64BABAA4F44A}">
-  <dimension ref="A4:N31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8636243C-025B-4E7E-AD67-64BABAA4F44A}">
+  <dimension ref="A4:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -711,9 +788,10 @@
     <col min="6" max="6" width="11.42578125" customWidth="1"/>
     <col min="7" max="7" width="11.5703125" customWidth="1"/>
     <col min="8" max="12" width="9.140625" customWidth="1"/>
+    <col min="14" max="14" width="29.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -750,8 +828,12 @@
       <c r="L4" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N4" t="str">
+        <f>D4&amp;" "&amp;F4&amp;" "&amp;H4&amp;" "&amp;J4&amp;" "&amp;L4</f>
+        <v>0.7s 120s/100% 32s 0.1 /</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -788,8 +870,12 @@
       <c r="L5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N5" t="str">
+        <f t="shared" ref="N5:N38" si="0">D5&amp;" "&amp;F5&amp;" "&amp;H5&amp;" "&amp;J5&amp;" "&amp;L5</f>
+        <v>0.7s 150s/100% 30s 0.1 /</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -826,8 +912,12 @@
       <c r="L6" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N6" t="str">
+        <f t="shared" si="0"/>
+        <v>0.7s 150s/72% 30s 0.1 /</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -864,8 +954,12 @@
       <c r="L7" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N7" t="str">
+        <f t="shared" si="0"/>
+        <v>0.7s 150s/100% 32s 0.1 /</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -902,8 +996,12 @@
       <c r="L8" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N8" t="str">
+        <f t="shared" si="0"/>
+        <v>0.7s 120s/100% 30s 0.1 /</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -940,8 +1038,12 @@
       <c r="L9" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N9" t="str">
+        <f t="shared" si="0"/>
+        <v>0.7s 300s/100% 32s 0.3 /</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -978,8 +1080,12 @@
       <c r="L10" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N10" t="str">
+        <f t="shared" si="0"/>
+        <v>0.7s 0s/100% 180s 0.2 1200s</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1016,8 +1122,12 @@
       <c r="L11" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N11" t="str">
+        <f t="shared" si="0"/>
+        <v>2s 600s/100% 120s 0.1 600s</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1054,8 +1164,12 @@
       <c r="L12" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N12" t="str">
+        <f t="shared" si="0"/>
+        <v>2s 300s/100% 120s 0.05 /</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1092,8 +1206,12 @@
       <c r="L13" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N13" t="str">
+        <f t="shared" si="0"/>
+        <v>0.7s 300s/100% 32s 0.1 /</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1130,8 +1248,12 @@
       <c r="L14" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N14" t="str">
+        <f t="shared" si="0"/>
+        <v>0.7s 0s/100% 16s 0.1 180s</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -1168,8 +1290,12 @@
       <c r="L15" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N15" t="str">
+        <f t="shared" si="0"/>
+        <v>0.7s 270s/100% 32s 0.1 600s</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -1205,6 +1331,10 @@
       </c>
       <c r="L16" t="s">
         <v>53</v>
+      </c>
+      <c r="N16" t="str">
+        <f t="shared" si="0"/>
+        <v>0.7s 30s/100% 32s 0.2 /</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -1244,6 +1374,10 @@
       <c r="L17" t="s">
         <v>53</v>
       </c>
+      <c r="N17" t="str">
+        <f t="shared" si="0"/>
+        <v>0.7s 60s/100% 30s 0.3 /</v>
+      </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -1282,6 +1416,10 @@
       <c r="L18" t="s">
         <v>53</v>
       </c>
+      <c r="N18" t="str">
+        <f t="shared" si="0"/>
+        <v>0.7s 300s/100% 60s 0.1 /</v>
+      </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -1320,6 +1458,10 @@
       <c r="L19" t="s">
         <v>53</v>
       </c>
+      <c r="N19" t="str">
+        <f t="shared" si="0"/>
+        <v>0.7s 900s/100% 30s 0.15 /</v>
+      </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -1358,6 +1500,10 @@
       <c r="L20" t="s">
         <v>53</v>
       </c>
+      <c r="N20" t="str">
+        <f t="shared" si="0"/>
+        <v>0.7s 32s/100% 32s 0.1 /</v>
+      </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -1396,6 +1542,10 @@
       <c r="L21" t="s">
         <v>53</v>
       </c>
+      <c r="N21" t="str">
+        <f t="shared" si="0"/>
+        <v>0.7s 120s/100% 32s 0.15 /</v>
+      </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -1434,6 +1584,10 @@
       <c r="L22" t="s">
         <v>57</v>
       </c>
+      <c r="N22" t="str">
+        <f t="shared" si="0"/>
+        <v>0.7s 300s/100% 90s 0.1 300s</v>
+      </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -1472,6 +1626,10 @@
       <c r="L23" t="s">
         <v>58</v>
       </c>
+      <c r="N23" t="str">
+        <f t="shared" si="0"/>
+        <v>0.7s 180s/100% 32s 0.1 120s</v>
+      </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
@@ -1511,8 +1669,9 @@
         <v>53</v>
       </c>
       <c r="M24" s="3"/>
-      <c r="N24" s="3" t="s">
-        <v>89</v>
+      <c r="N24" t="str">
+        <f t="shared" si="0"/>
+        <v>0.7s 180s/100% 32s 0.15 /</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
@@ -1552,6 +1711,10 @@
       <c r="L25" t="s">
         <v>53</v>
       </c>
+      <c r="N25" t="str">
+        <f t="shared" si="0"/>
+        <v>0.7s 180s/100% 32s 0.1 /</v>
+      </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -1590,6 +1753,10 @@
       <c r="L26" t="s">
         <v>53</v>
       </c>
+      <c r="N26" t="str">
+        <f t="shared" si="0"/>
+        <v>5s 180s/100% 32s 0.1 /</v>
+      </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -1628,6 +1795,10 @@
       <c r="L27" t="s">
         <v>53</v>
       </c>
+      <c r="N27" t="str">
+        <f t="shared" si="0"/>
+        <v>0.7s 300s/80% 32s 0.2 /</v>
+      </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -1666,6 +1837,10 @@
       <c r="L28" t="s">
         <v>59</v>
       </c>
+      <c r="N28" t="str">
+        <f t="shared" si="0"/>
+        <v>0.7s 300s/100% 32s 0.1 7200s</v>
+      </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
@@ -1704,13 +1879,17 @@
       <c r="L29" t="s">
         <v>85</v>
       </c>
+      <c r="N29" t="str">
+        <f t="shared" si="0"/>
+        <v>0.7s 300s/100% 32s 0.1 1800s</v>
+      </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>86</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>48</v>
@@ -1742,21 +1921,146 @@
       <c r="L30" t="s">
         <v>87</v>
       </c>
+      <c r="N30" t="str">
+        <f t="shared" si="0"/>
+        <v>0.7s 120s/100% 32s 0 0s</v>
+      </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B31" s="2"/>
+      <c r="A31" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D31" t="s">
+        <v>90</v>
+      </c>
+      <c r="E31" t="s">
+        <v>49</v>
+      </c>
+      <c r="F31" t="s">
+        <v>66</v>
+      </c>
+      <c r="G31" t="s">
+        <v>50</v>
+      </c>
+      <c r="H31" t="s">
+        <v>62</v>
+      </c>
+      <c r="I31" t="s">
+        <v>51</v>
+      </c>
+      <c r="J31" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="K31" t="s">
+        <v>52</v>
+      </c>
+      <c r="L31" t="s">
+        <v>53</v>
+      </c>
+      <c r="N31" t="str">
+        <f t="shared" si="0"/>
+        <v>5.0s 300s/100% 32s 0.1 /</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D32" t="s">
+        <v>93</v>
+      </c>
+      <c r="E32" t="s">
+        <v>49</v>
+      </c>
+      <c r="F32" t="s">
+        <v>94</v>
+      </c>
+      <c r="G32" t="s">
+        <v>50</v>
+      </c>
+      <c r="H32" t="s">
+        <v>95</v>
+      </c>
+      <c r="I32" t="s">
+        <v>51</v>
+      </c>
+      <c r="J32" t="s">
+        <v>96</v>
+      </c>
+      <c r="K32" t="s">
+        <v>52</v>
+      </c>
+      <c r="L32" t="s">
+        <v>85</v>
+      </c>
+      <c r="N32" t="str">
+        <f>D32&amp;" "&amp;F32&amp;" "&amp;H32&amp;" "&amp;J32&amp;" "&amp;L32</f>
+        <v>0.7s, 60s/100%, 2s, 10%, 1800s</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N33" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    </v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" s="5"/>
+      <c r="B34" s="2"/>
+      <c r="J34" s="1"/>
+      <c r="N34" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    </v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N35" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    </v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N36" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    </v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N37" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    </v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N38" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    </v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="B1:B30 B32:B1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+  <conditionalFormatting sqref="B1:B30 B33:B1048576">
+    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  <conditionalFormatting sqref="B1:B31 B33:B1048576">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C30">
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+  <conditionalFormatting sqref="N4:N38">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update to 3.0 version with config file. Now only few files use it though.
Also, preparation for config.py file, that would hold few of the data together for quicker updates and distinction of corridor boxes, for now, there are 2 and extra 1 "unit" on my table
</commit_message>
<xml_diff>
--- a/HELPMEfile - MANUAL/tabulka programu.xlsx
+++ b/HELPMEfile - MANUAL/tabulka programu.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\novak\Documents\GitHub\LuxMeter\HELPMEfile - MANUAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6642B214-3968-4C95-8B38-59373A7ECF18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C3D704C-7186-47AF-A5DC-4D4D1DD4B54B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="109">
   <si>
     <t>body pro vyplneni a postupne se bude "filtrovat seznam" mereni a když bude prazdne, tak tlacitko zalozit a pripravil by se novy program a cislo? + fajfka jestli je k tomu uz vytvoreny testovaci program?</t>
   </si>
@@ -352,20 +352,74 @@
     <t>2s,</t>
   </si>
   <si>
-    <t>10%,</t>
-  </si>
-  <si>
     <t>Program č. 29</t>
   </si>
   <si>
     <t>FIN:5s, RON:300s/100%, FOUT:32s, ABL:10%, SOFF:/</t>
+  </si>
+  <si>
+    <t>REGENT</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ty </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>modré</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> texty musí zákazník/obchodník definovat. Jinak si to akorát můžeme domýšlet.</t>
+    </r>
+  </si>
+  <si>
+    <t>FIN:0.7s, RON:300s/100%, FOUT:1s, ABL:30%, SOFF:/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FOUT</t>
+  </si>
+  <si>
+    <t>1s</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SOFF</t>
+  </si>
+  <si>
+    <t>Program č. 30</t>
+  </si>
+  <si>
+    <t>Program č. 31</t>
+  </si>
+  <si>
+    <t>FIN:5s, RON:600s/100%, FOUT:32s, ABL:10%, SOFF:/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RON</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ABL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -414,6 +468,15 @@
       <name val="Tahoma"/>
       <family val="2"/>
       <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -489,6 +552,72 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="Displaying Corridor - základní na...">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E17B749-81AD-EA33-C7DE-6D3F5FE0A1C1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="647700" y="1790700"/>
+          <a:ext cx="4181475" cy="2295525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -754,10 +883,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2"/>
+  <dimension ref="B2:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -767,17 +896,23 @@
         <v>0</v>
       </c>
     </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>99</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8636243C-025B-4E7E-AD67-64BABAA4F44A}">
-  <dimension ref="A4:N38"/>
+  <dimension ref="A4:P41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -791,7 +926,7 @@
     <col min="14" max="14" width="29.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -833,7 +968,7 @@
         <v>0.7s 120s/100% 32s 0.1 /</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -871,11 +1006,11 @@
         <v>53</v>
       </c>
       <c r="N5" t="str">
-        <f t="shared" ref="N5:N38" si="0">D5&amp;" "&amp;F5&amp;" "&amp;H5&amp;" "&amp;J5&amp;" "&amp;L5</f>
+        <f t="shared" ref="N5:N41" si="0">D5&amp;" "&amp;F5&amp;" "&amp;H5&amp;" "&amp;J5&amp;" "&amp;L5</f>
         <v>0.7s 150s/100% 30s 0.1 /</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -917,7 +1052,7 @@
         <v>0.7s 150s/72% 30s 0.1 /</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -958,8 +1093,11 @@
         <f t="shared" si="0"/>
         <v>0.7s 150s/100% 32s 0.1 /</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1001,7 +1139,7 @@
         <v>0.7s 120s/100% 30s 0.1 /</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1043,7 +1181,7 @@
         <v>0.7s 300s/100% 32s 0.3 /</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1085,7 +1223,7 @@
         <v>0.7s 0s/100% 180s 0.2 1200s</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1127,7 +1265,7 @@
         <v>2s 600s/100% 120s 0.1 600s</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1169,7 +1307,7 @@
         <v>2s 300s/100% 120s 0.05 /</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1211,7 +1349,7 @@
         <v>0.7s 300s/100% 32s 0.1 /</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1253,7 +1391,7 @@
         <v>0.7s 0s/100% 16s 0.1 180s</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -1295,7 +1433,7 @@
         <v>0.7s 270s/100% 32s 0.1 600s</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -1337,7 +1475,7 @@
         <v>0.7s 30s/100% 32s 0.2 /</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -1379,7 +1517,7 @@
         <v>0.7s 60s/100% 30s 0.3 /</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -1421,7 +1559,7 @@
         <v>0.7s 300s/100% 60s 0.1 /</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -1463,7 +1601,7 @@
         <v>0.7s 900s/100% 30s 0.15 /</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -1505,7 +1643,7 @@
         <v>0.7s 32s/100% 32s 0.1 /</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -1547,7 +1685,7 @@
         <v>0.7s 120s/100% 32s 0.15 /</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>37</v>
       </c>
@@ -1589,7 +1727,7 @@
         <v>0.7s 300s/100% 90s 0.1 300s</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>39</v>
       </c>
@@ -1631,7 +1769,7 @@
         <v>0.7s 180s/100% 32s 0.1 120s</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>41</v>
       </c>
@@ -1674,7 +1812,7 @@
         <v>0.7s 180s/100% 32s 0.15 /</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -1716,7 +1854,7 @@
         <v>0.7s 180s/100% 32s 0.1 /</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>44</v>
       </c>
@@ -1758,7 +1896,7 @@
         <v>5s 180s/100% 32s 0.1 /</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>45</v>
       </c>
@@ -1800,7 +1938,7 @@
         <v>0.7s 300s/80% 32s 0.2 /</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>46</v>
       </c>
@@ -1842,7 +1980,7 @@
         <v>0.7s 300s/100% 32s 0.1 7200s</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>83</v>
       </c>
@@ -1884,7 +2022,7 @@
         <v>0.7s 300s/100% 32s 0.1 1800s</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>86</v>
       </c>
@@ -1925,13 +2063,16 @@
         <f t="shared" si="0"/>
         <v>0.7s 120s/100% 32s 0 0s</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P30" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>91</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>48</v>
@@ -1968,9 +2109,9 @@
         <v>5.0s 300s/100% 32s 0.1 /</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>92</v>
@@ -1996,8 +2137,8 @@
       <c r="I32" t="s">
         <v>51</v>
       </c>
-      <c r="J32" t="s">
-        <v>96</v>
+      <c r="J32" s="1">
+        <v>0.1</v>
       </c>
       <c r="K32" t="s">
         <v>52</v>
@@ -2007,22 +2148,91 @@
       </c>
       <c r="N32" t="str">
         <f>D32&amp;" "&amp;F32&amp;" "&amp;H32&amp;" "&amp;J32&amp;" "&amp;L32</f>
-        <v>0.7s, 60s/100%, 2s, 10%, 1800s</v>
+        <v>0.7s, 60s/100%, 2s, 0.1 1800s</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D33" t="s">
+        <v>60</v>
+      </c>
+      <c r="E33" t="s">
+        <v>49</v>
+      </c>
+      <c r="F33" t="s">
+        <v>66</v>
+      </c>
+      <c r="G33" t="s">
+        <v>101</v>
+      </c>
+      <c r="H33" t="s">
+        <v>102</v>
+      </c>
+      <c r="I33" t="s">
+        <v>51</v>
+      </c>
+      <c r="J33" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="K33" t="s">
+        <v>103</v>
+      </c>
+      <c r="L33" t="s">
+        <v>53</v>
+      </c>
       <c r="N33" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    </v>
+        <v>0.7s 300s/100% 1s 0.3 /</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
-      <c r="B34" s="2"/>
-      <c r="J34" s="1"/>
+      <c r="A34" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D34" t="s">
+        <v>80</v>
+      </c>
+      <c r="E34" t="s">
+        <v>107</v>
+      </c>
+      <c r="F34" t="s">
+        <v>69</v>
+      </c>
+      <c r="G34" t="s">
+        <v>101</v>
+      </c>
+      <c r="H34" t="s">
+        <v>62</v>
+      </c>
+      <c r="I34" t="s">
+        <v>108</v>
+      </c>
+      <c r="J34" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="K34" t="s">
+        <v>103</v>
+      </c>
+      <c r="L34" t="s">
+        <v>53</v>
+      </c>
       <c r="N34" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    </v>
+        <v>5s 600s/100% 32s 0.1 /</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
@@ -2049,15 +2259,33 @@
         <v xml:space="preserve">    </v>
       </c>
     </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N39" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    </v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N40" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    </v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N41" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    </v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="B1:B30 B33:B1048576">
+  <conditionalFormatting sqref="B1:B30 B35:B1048576">
     <cfRule type="duplicateValues" dxfId="2" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B31 B33:B1048576">
+  <conditionalFormatting sqref="B1:B31 B35:B1048576">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N4:N38">
+  <conditionalFormatting sqref="N4:N41">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>